<commit_message>
cambios a mayo de 2023
</commit_message>
<xml_diff>
--- a/src/assets/datos_generales.xlsx
+++ b/src/assets/datos_generales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cencarnacion\develop\timbrado\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cencarnacion\develop\timbrado_js\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC09AD9-386D-4403-87E6-DC95AF1CCF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDB767D-D555-4F20-93A5-99C3C4AFE664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t>CFDI 3.2</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>SEGURIDAD_SOCIAL</t>
+  </si>
+  <si>
+    <t>CP_RECEPTOR</t>
+  </si>
+  <si>
+    <t>HORARIO</t>
   </si>
 </sst>
 </file>
@@ -419,64 +425,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -876,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN4"/>
+  <dimension ref="A1:BP4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB5" sqref="A5:XFD264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -946,9 +948,12 @@
     <col min="64" max="64" width="15" customWidth="1"/>
     <col min="65" max="65" width="28.42578125" customWidth="1"/>
     <col min="66" max="66" width="21.140625" customWidth="1"/>
+    <col min="67" max="67" width="20.85546875" customWidth="1"/>
+    <col min="68" max="68" width="32.42578125" customWidth="1"/>
+    <col min="69" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1021,7 @@
       <c r="BI1" s="16"/>
       <c r="BJ1" s="16"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1111,7 @@
       <c r="BI2" s="18"/>
       <c r="BJ2" s="18"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1142,7 @@
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3" t="s">
@@ -1158,7 +1163,7 @@
       <c r="Q3" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" t="s">
         <v>15</v>
       </c>
       <c r="S3" t="s">
@@ -1167,337 +1172,349 @@
       <c r="T3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="U3" t="s">
         <v>15</v>
       </c>
       <c r="V3" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AU3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AX3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="BC3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BD3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="BF3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BG3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BI3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BJ3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BK3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BL3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BN3" s="21" t="s">
+      <c r="W3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BD3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="BF3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BG3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BI3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BJ3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="BP3" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:66" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="26" t="s">
+      <c r="S4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="U4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="26" t="s">
+      <c r="W4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="X4" s="26" t="s">
+      <c r="X4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="Y4" s="26" t="s">
+      <c r="Y4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA4" s="26" t="s">
+      <c r="AA4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AB4" s="27" t="s">
+      <c r="AB4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AC4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AD4" s="23" t="s">
+      <c r="AD4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AE4" s="26" t="s">
+      <c r="AE4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AF4" s="26" t="s">
+      <c r="AF4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AI4" s="27" t="s">
+      <c r="AI4" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="AJ4" s="23" t="s">
+      <c r="AJ4" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AK4" s="26" t="s">
+      <c r="AK4" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="AL4" s="26" t="s">
+      <c r="AL4" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="AM4" s="25" t="s">
+      <c r="AM4" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AN4" s="26" t="s">
+      <c r="AN4" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AO4" s="26" t="s">
+      <c r="AO4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AP4" s="26" t="s">
+      <c r="AP4" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AQ4" s="23" t="s">
+      <c r="AQ4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AR4" s="23" t="s">
+      <c r="AR4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AS4" s="26" t="s">
+      <c r="AS4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AT4" s="26" t="s">
+      <c r="AT4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="AU4" s="23" t="s">
+      <c r="AU4" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AV4" s="25" t="s">
+      <c r="AV4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AW4" s="23" t="s">
+      <c r="AW4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="AX4" s="23" t="s">
+      <c r="AX4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AY4" s="23" t="s">
+      <c r="AY4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AZ4" s="23" t="s">
+      <c r="AZ4" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BA4" s="23" t="s">
+      <c r="BA4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="BB4" s="23" t="s">
+      <c r="BB4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="BC4" s="23" t="s">
+      <c r="BC4" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="BD4" s="25" t="s">
+      <c r="BD4" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="BE4" s="23" t="s">
+      <c r="BE4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="BF4" s="26" t="s">
+      <c r="BF4" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="BG4" s="26" t="s">
+      <c r="BG4" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="BH4" s="26" t="s">
+      <c r="BH4" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BI4" s="26" t="s">
+      <c r="BI4" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="BJ4" s="26" t="s">
+      <c r="BJ4" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BK4" s="26" t="s">
+      <c r="BK4" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BL4" s="26" t="s">
+      <c r="BL4" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BM4" s="26" t="s">
+      <c r="BM4" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="BN4" s="26" t="s">
+      <c r="BN4" s="24" t="s">
         <v>80</v>
+      </c>
+      <c r="BO4" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="BP4" s="24" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>